<commit_message>
Updated data in light of fix_baddata_wip
</commit_message>
<xml_diff>
--- a/debug/master_baddata.xlsx
+++ b/debug/master_baddata.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbhilga\GitHub\vg-dissertation\debug\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
   </bookViews>
@@ -22,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="64">
   <si>
     <t>Subject</t>
   </si>
@@ -186,14 +181,49 @@
     <t>rating6</t>
   </si>
   <si>
-    <t>CONFLICT!</t>
+    <t>BAD</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BAD</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BAD</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BAD</t>
+  </si>
+  <si>
+    <t>Maybe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +356,13 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -985,7 +1022,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -995,17 +1032,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="1350" ySplit="600" topLeftCell="N1" activePane="bottomRight"/>
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1350" ySplit="600" activePane="bottomRight"/>
+      <selection activeCell="M19" sqref="M19:N20"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="P6" sqref="P6"/>
+      <selection pane="bottomRight" activeCell="W51" sqref="W51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1169,15 +1206,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54">
       <c r="A2">
         <v>33</v>
       </c>
-      <c r="N2">
-        <v>-999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54">
       <c r="A3">
         <v>63</v>
       </c>
@@ -1200,7 +1237,7 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54">
       <c r="A4">
         <v>82</v>
       </c>
@@ -1223,7 +1260,7 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54">
       <c r="A5">
         <v>140</v>
       </c>
@@ -1246,682 +1283,691 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54">
       <c r="A6">
         <v>168</v>
       </c>
-      <c r="C6">
-        <v>-999</v>
-      </c>
-      <c r="E6">
-        <v>-999</v>
-      </c>
-      <c r="F6">
-        <v>-999</v>
-      </c>
-      <c r="G6">
-        <v>-999</v>
-      </c>
-      <c r="I6">
-        <v>-999</v>
-      </c>
-      <c r="J6">
-        <v>-999</v>
-      </c>
-      <c r="K6">
-        <v>-999</v>
-      </c>
-      <c r="N6">
-        <v>-999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54">
       <c r="A7">
         <v>170</v>
       </c>
       <c r="N7">
-        <v>-999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54">
       <c r="A8">
         <v>309</v>
       </c>
       <c r="AV8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54">
       <c r="A9">
         <v>310</v>
       </c>
       <c r="AV9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:54">
       <c r="A10">
         <v>311</v>
       </c>
       <c r="AV10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54">
       <c r="A11">
         <v>312</v>
       </c>
       <c r="AV11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54">
       <c r="A12">
         <v>313</v>
       </c>
       <c r="AV12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54">
       <c r="A13">
         <v>314</v>
       </c>
       <c r="AV13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:54">
       <c r="A14">
         <v>316</v>
       </c>
       <c r="AV14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:54">
       <c r="A15">
         <v>317</v>
       </c>
       <c r="AV15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:54">
       <c r="A16">
         <v>318</v>
       </c>
       <c r="AV16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:48">
       <c r="A17">
         <v>319</v>
       </c>
       <c r="AV17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:48">
       <c r="A18">
         <v>320</v>
       </c>
       <c r="AV18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:48">
       <c r="A19">
         <v>321</v>
       </c>
       <c r="AV19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:48">
       <c r="A20">
         <v>322</v>
       </c>
       <c r="AV20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:48">
       <c r="A21">
         <v>323</v>
       </c>
       <c r="AV21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:48">
       <c r="A22">
         <v>324</v>
       </c>
       <c r="AV22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:48">
       <c r="A23">
         <v>326</v>
       </c>
       <c r="AV23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:48">
       <c r="A24">
         <v>328</v>
       </c>
       <c r="V24">
-        <v>-999</v>
+        <v>4</v>
       </c>
       <c r="W24">
-        <v>-999</v>
+        <v>3</v>
       </c>
       <c r="X24">
-        <v>-999</v>
+        <v>5</v>
       </c>
       <c r="Y24">
-        <v>-999</v>
+        <v>3</v>
       </c>
       <c r="Z24">
-        <v>-999</v>
+        <v>5</v>
       </c>
       <c r="AD24">
-        <v>-999</v>
+        <v>4</v>
       </c>
       <c r="AF24">
-        <v>-999</v>
+        <v>3</v>
       </c>
       <c r="AH24">
-        <v>-999</v>
+        <v>5</v>
       </c>
       <c r="AI24">
-        <v>-999</v>
+        <v>3</v>
       </c>
       <c r="AK24">
-        <v>-999</v>
+        <v>5</v>
       </c>
       <c r="AV24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:48">
       <c r="A25">
         <v>329</v>
       </c>
       <c r="AV25" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:48">
       <c r="A26">
         <v>330</v>
       </c>
       <c r="AV26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:48">
       <c r="A27">
         <v>331</v>
       </c>
       <c r="AV27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:48">
       <c r="A28">
         <v>332</v>
       </c>
       <c r="AV28" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:48">
       <c r="A29">
         <v>333</v>
       </c>
       <c r="AV29" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:48" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:48">
       <c r="A30">
         <v>334</v>
       </c>
       <c r="AV30" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:48" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:48">
       <c r="A31">
         <v>335</v>
       </c>
       <c r="AV31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:48">
       <c r="A32">
         <v>336</v>
       </c>
       <c r="AV32" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:48">
       <c r="A33">
         <v>337</v>
       </c>
       <c r="AV33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:48">
       <c r="A34">
         <v>338</v>
       </c>
       <c r="AV34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:48" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:48">
       <c r="A35">
         <v>339</v>
       </c>
       <c r="AV35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:48">
       <c r="A36">
         <v>340</v>
       </c>
       <c r="AV36" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:48" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:48">
       <c r="A37">
         <v>342</v>
       </c>
       <c r="AV37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:48">
       <c r="A38">
         <v>343</v>
       </c>
       <c r="AG38">
-        <v>-999</v>
+        <v>1</v>
       </c>
       <c r="AV38" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:48" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:48">
       <c r="A39">
         <v>344</v>
       </c>
       <c r="AR39">
-        <v>-999</v>
+        <v>18</v>
       </c>
       <c r="AS39">
-        <v>-999</v>
+        <v>5</v>
       </c>
       <c r="AT39">
-        <v>-999</v>
+        <v>1</v>
       </c>
       <c r="AV39" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:48" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:48">
       <c r="A40">
         <v>345</v>
       </c>
       <c r="AV40" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="41" spans="1:48" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:48">
       <c r="A41">
         <v>346</v>
       </c>
       <c r="AV41" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:48" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:48">
       <c r="A42">
         <v>347</v>
       </c>
       <c r="AV42" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="43" spans="1:48" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:48">
       <c r="A43">
         <v>348</v>
       </c>
       <c r="AV43" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:48">
       <c r="A44">
         <v>349</v>
       </c>
       <c r="AV44" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" spans="1:48" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:48">
       <c r="A45">
         <v>350</v>
       </c>
       <c r="AV45" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:48" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:48">
       <c r="A46">
         <v>351</v>
       </c>
       <c r="AV46" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="47" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:48">
       <c r="A47">
         <v>352</v>
       </c>
       <c r="AV47" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="48" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:48">
       <c r="A48">
         <v>353</v>
       </c>
       <c r="AV48" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="49" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:48">
       <c r="A49">
         <v>354</v>
       </c>
       <c r="AV49" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="50" spans="1:48" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:48">
       <c r="A50">
         <v>355</v>
       </c>
-      <c r="W50">
-        <v>-999</v>
+      <c r="W50" t="s">
+        <v>62</v>
       </c>
       <c r="AV50" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="51" spans="1:48" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:48">
       <c r="A51">
         <v>356</v>
       </c>
       <c r="AV51" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="52" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:48">
       <c r="A52">
         <v>357</v>
       </c>
       <c r="AV52" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:48">
       <c r="A53">
         <v>358</v>
       </c>
       <c r="AV53" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="54" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:48">
       <c r="A54">
         <v>359</v>
       </c>
       <c r="S54">
-        <v>-999</v>
+        <v>3</v>
       </c>
       <c r="AV54" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:48">
       <c r="A55">
         <v>360</v>
       </c>
       <c r="AV55" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:48" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:48">
       <c r="A56">
         <v>361</v>
       </c>
       <c r="AV56" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:48" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:48">
       <c r="A57">
         <v>362</v>
       </c>
       <c r="AV57" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="58" spans="1:48" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:48">
       <c r="A58">
         <v>365</v>
       </c>
-      <c r="B58">
-        <v>-999</v>
-      </c>
-      <c r="C58">
-        <v>-999</v>
-      </c>
-      <c r="D58">
-        <v>-999</v>
-      </c>
-      <c r="H58">
-        <v>-999</v>
+      <c r="B58" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" t="s">
+        <v>62</v>
+      </c>
+      <c r="D58" t="s">
+        <v>62</v>
+      </c>
+      <c r="E58" t="s">
+        <v>62</v>
+      </c>
+      <c r="F58" t="s">
+        <v>62</v>
+      </c>
+      <c r="G58" t="s">
+        <v>62</v>
+      </c>
+      <c r="H58" t="s">
+        <v>62</v>
       </c>
       <c r="O58">
-        <v>-999</v>
+        <v>3</v>
       </c>
       <c r="P58">
-        <v>-999</v>
+        <v>1</v>
       </c>
       <c r="Q58">
-        <v>-999</v>
+        <v>6</v>
       </c>
       <c r="R58">
-        <v>-999</v>
+        <v>3</v>
       </c>
       <c r="V58">
-        <v>-999</v>
+        <v>6</v>
       </c>
       <c r="W58">
-        <v>-999</v>
+        <v>6</v>
       </c>
       <c r="X58">
-        <v>-999</v>
+        <v>2</v>
       </c>
       <c r="Y58">
-        <v>-999</v>
+        <v>3</v>
       </c>
       <c r="AA58">
-        <v>-999</v>
+        <v>4</v>
       </c>
       <c r="AB58">
-        <v>-999</v>
+        <v>5</v>
       </c>
       <c r="AC58">
-        <v>-999</v>
+        <v>5</v>
       </c>
       <c r="AD58">
-        <v>-999</v>
+        <v>2</v>
       </c>
       <c r="AE58">
-        <v>-999</v>
+        <v>2</v>
       </c>
       <c r="AF58">
-        <v>-999</v>
+        <v>3</v>
       </c>
       <c r="AG58">
-        <v>-999</v>
+        <v>4</v>
       </c>
       <c r="AI58">
-        <v>-999</v>
+        <v>3</v>
       </c>
       <c r="AJ58">
-        <v>-999</v>
+        <v>5</v>
       </c>
       <c r="AK58">
-        <v>-999</v>
+        <v>5</v>
       </c>
       <c r="AL58">
-        <v>-999</v>
+        <v>4</v>
       </c>
       <c r="AM58">
-        <v>-999</v>
+        <v>6</v>
       </c>
       <c r="AN58">
-        <v>-999</v>
+        <v>6</v>
       </c>
       <c r="AO58">
-        <v>-999</v>
+        <v>5</v>
       </c>
       <c r="AP58">
-        <v>-999</v>
+        <v>3</v>
       </c>
       <c r="AR58">
-        <v>-999</v>
+        <v>19</v>
       </c>
       <c r="AU58">
-        <v>-999</v>
-      </c>
-    </row>
-    <row r="59" spans="1:48" x14ac:dyDescent="0.25">
+        <v>3.82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:48">
       <c r="A59">
         <v>367</v>
       </c>
       <c r="F59">
-        <v>-999</v>
+        <v>1</v>
       </c>
       <c r="I59">
-        <v>-999</v>
+        <v>0</v>
       </c>
       <c r="K59">
-        <v>-999</v>
+        <v>2</v>
       </c>
       <c r="L59" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="M59" t="s">
-        <v>54</v>
-      </c>
-      <c r="R59">
-        <v>-999</v>
-      </c>
-      <c r="T59">
-        <v>-999</v>
-      </c>
-      <c r="U59">
-        <v>-999</v>
-      </c>
-      <c r="V59">
-        <v>-999</v>
-      </c>
-      <c r="W59">
-        <v>-999</v>
-      </c>
-      <c r="Y59">
-        <v>-999</v>
-      </c>
-      <c r="Z59">
-        <v>-999</v>
-      </c>
-      <c r="AA59">
-        <v>-999</v>
-      </c>
-      <c r="AB59">
-        <v>-999</v>
-      </c>
-      <c r="AC59">
-        <v>-999</v>
-      </c>
-      <c r="AD59">
-        <v>-999</v>
-      </c>
-      <c r="AE59">
-        <v>-999</v>
-      </c>
-      <c r="AF59">
-        <v>-999</v>
-      </c>
-      <c r="AG59">
-        <v>-999</v>
-      </c>
-      <c r="AH59">
-        <v>-999</v>
-      </c>
-      <c r="AI59">
-        <v>-999</v>
-      </c>
-      <c r="AJ59">
-        <v>-999</v>
-      </c>
-      <c r="AK59">
-        <v>-999</v>
-      </c>
-      <c r="AL59">
-        <v>-999</v>
-      </c>
-      <c r="AM59">
-        <v>-999</v>
-      </c>
-      <c r="AO59">
-        <v>-999</v>
-      </c>
-      <c r="AP59">
-        <v>-999</v>
-      </c>
-      <c r="AQ59">
-        <v>-999</v>
-      </c>
-      <c r="AR59">
-        <v>-999</v>
-      </c>
-      <c r="AS59">
-        <v>-999</v>
-      </c>
-      <c r="AT59">
-        <v>-999</v>
-      </c>
-      <c r="AU59">
-        <v>-999</v>
+        <v>63</v>
+      </c>
+      <c r="R59" t="s">
+        <v>62</v>
+      </c>
+      <c r="T59" t="s">
+        <v>62</v>
+      </c>
+      <c r="U59" t="s">
+        <v>62</v>
+      </c>
+      <c r="V59" t="s">
+        <v>62</v>
+      </c>
+      <c r="W59" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT59" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU59" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1930,6 +1976,8 @@
       <sortCondition ref="A1:A59"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>